<commit_message>
webpage update + eplainer notebook
</commit_message>
<xml_diff>
--- a/notebooks/Data/Rogue_One_A_Star_Wars_Story/centrality.xlsx
+++ b/notebooks/Data/Rogue_One_A_Star_Wars_Story/centrality.xlsx
@@ -130,412 +130,412 @@
     <t>Ralo Surrel</t>
   </si>
   <si>
+    <t>Saw Gerrera</t>
+  </si>
+  <si>
+    <t>Unidentified Human Rebel (Profundity)</t>
+  </si>
+  <si>
+    <t>Shollan</t>
+  </si>
+  <si>
+    <t>Jaldine Gerams</t>
+  </si>
+  <si>
+    <t>Taidu Sefla</t>
+  </si>
+  <si>
+    <t>Tobix Chasser</t>
+  </si>
+  <si>
+    <t>Zal Dinnes</t>
+  </si>
+  <si>
+    <t>Nesta Term</t>
+  </si>
+  <si>
+    <t>DT-5537</t>
+  </si>
+  <si>
+    <t>Jan Dodonna</t>
+  </si>
+  <si>
+    <t>Baccam Grafis</t>
+  </si>
+  <si>
+    <t>Obi-Wan Kenobi</t>
+  </si>
+  <si>
+    <t>Harb Binli</t>
+  </si>
+  <si>
+    <t>R2-D2</t>
+  </si>
+  <si>
+    <t>Bistan</t>
+  </si>
+  <si>
+    <t>Robich Duggsin</t>
+  </si>
+  <si>
+    <t>Feyn Vann</t>
+  </si>
+  <si>
+    <t>Omisha Joyo</t>
+  </si>
+  <si>
+    <t>Garn Stewer</t>
+  </si>
+  <si>
+    <t>Nozzo Naytaan</t>
+  </si>
+  <si>
+    <t>Wilhuff Tarkin</t>
+  </si>
+  <si>
+    <t>Rasett Milio</t>
+  </si>
+  <si>
+    <t>Paodok'Draba'Takat</t>
+  </si>
+  <si>
+    <t>Sa'Kalla</t>
+  </si>
+  <si>
+    <t>Bodhi Rook</t>
+  </si>
+  <si>
+    <t>Ames Uravan</t>
+  </si>
+  <si>
+    <t>Nower Jebel</t>
+  </si>
+  <si>
+    <t>Toshdor Ni</t>
+  </si>
+  <si>
+    <t>C-3PO</t>
+  </si>
+  <si>
+    <t>KMD-RA-71</t>
+  </si>
+  <si>
+    <t>Woan Barso</t>
+  </si>
+  <si>
+    <t>C2-B5</t>
+  </si>
+  <si>
+    <t>Raymus Antilles</t>
+  </si>
+  <si>
+    <t>K-2SO</t>
+  </si>
+  <si>
     <t>Edrio</t>
   </si>
   <si>
-    <t>Saw Gerrera</t>
-  </si>
-  <si>
-    <t>Unidentified Human Rebel (Profundity)</t>
-  </si>
-  <si>
-    <t>Shollan</t>
-  </si>
-  <si>
-    <t>Jaldine Gerams</t>
-  </si>
-  <si>
-    <t>Taidu Sefla</t>
-  </si>
-  <si>
-    <t>Tobix Chasser</t>
-  </si>
-  <si>
-    <t>Zal Dinnes</t>
-  </si>
-  <si>
-    <t>Nesta Term</t>
-  </si>
-  <si>
-    <t>DT-5537</t>
-  </si>
-  <si>
-    <t>Jan Dodonna</t>
-  </si>
-  <si>
-    <t>Baccam Grafis</t>
-  </si>
-  <si>
-    <t>Obi-Wan Kenobi</t>
-  </si>
-  <si>
-    <t>Harb Binli</t>
-  </si>
-  <si>
-    <t>R2-D2</t>
-  </si>
-  <si>
-    <t>Bistan</t>
-  </si>
-  <si>
-    <t>Robich Duggsin</t>
-  </si>
-  <si>
-    <t>Feyn Vann</t>
-  </si>
-  <si>
-    <t>Omisha Joyo</t>
-  </si>
-  <si>
-    <t>Garn Stewer</t>
-  </si>
-  <si>
-    <t>Nozzo Naytaan</t>
-  </si>
-  <si>
-    <t>Wilhuff Tarkin</t>
-  </si>
-  <si>
-    <t>Rasett Milio</t>
-  </si>
-  <si>
-    <t>Paodok'Draba'Takat</t>
-  </si>
-  <si>
-    <t>Sa'Kalla</t>
-  </si>
-  <si>
-    <t>Bodhi Rook</t>
-  </si>
-  <si>
-    <t>Ames Uravan</t>
-  </si>
-  <si>
-    <t>Nower Jebel</t>
-  </si>
-  <si>
-    <t>Toshdor Ni</t>
-  </si>
-  <si>
-    <t>C-3PO</t>
-  </si>
-  <si>
-    <t>KMD-RA-71</t>
-  </si>
-  <si>
-    <t>Woan Barso</t>
-  </si>
-  <si>
-    <t>C2-B5</t>
-  </si>
-  <si>
-    <t>Raymus Antilles</t>
-  </si>
-  <si>
-    <t>K-2SO</t>
+    <t>Unidentified Blue Squadron pilot</t>
+  </si>
+  <si>
+    <t>Unidentified Tantive IV pilot</t>
+  </si>
+  <si>
+    <t>Gale Torg</t>
+  </si>
+  <si>
+    <t>Sirro Argonne</t>
+  </si>
+  <si>
+    <t>Unidentified fleet trooper</t>
+  </si>
+  <si>
+    <t>Namen Takamen</t>
+  </si>
+  <si>
+    <t>Danbit Brun</t>
+  </si>
+  <si>
+    <t>Dobias Cole-Truten</t>
+  </si>
+  <si>
+    <t>Killi Gimm</t>
+  </si>
+  <si>
+    <t>Serchill Rostok</t>
+  </si>
+  <si>
+    <t>Torius Chord</t>
+  </si>
+  <si>
+    <t>Attico Wred</t>
+  </si>
+  <si>
+    <t>TK-14057</t>
+  </si>
+  <si>
+    <t>Jek Tono Porkins</t>
+  </si>
+  <si>
+    <t>Casido</t>
+  </si>
+  <si>
+    <t>Dunstig Pterro</t>
+  </si>
+  <si>
+    <t>Datchi Creel</t>
+  </si>
+  <si>
+    <t>Bandwin Cor</t>
+  </si>
+  <si>
+    <t>R3-M2</t>
+  </si>
+  <si>
+    <t>Riss Clyos</t>
+  </si>
+  <si>
+    <t>Tivik</t>
+  </si>
+  <si>
+    <t>Farsin Kappehl</t>
+  </si>
+  <si>
+    <t>Gavra Ubrento</t>
+  </si>
+  <si>
+    <t>Has Obitt</t>
+  </si>
+  <si>
+    <t>Garven Dreis</t>
+  </si>
+  <si>
+    <t>Niles Gavla</t>
+  </si>
+  <si>
+    <t>Chirrut Îmwe</t>
+  </si>
+  <si>
+    <t>Farns Monsbee</t>
   </si>
   <si>
     <t>Pendra Siliu</t>
   </si>
   <si>
-    <t>Unidentified Blue Squadron pilot</t>
-  </si>
-  <si>
-    <t>Unidentified Tantive IV pilot</t>
-  </si>
-  <si>
-    <t>Gale Torg</t>
-  </si>
-  <si>
-    <t>Sirro Argonne</t>
-  </si>
-  <si>
-    <t>Unidentified fleet trooper</t>
-  </si>
-  <si>
-    <t>Namen Takamen</t>
-  </si>
-  <si>
-    <t>Danbit Brun</t>
-  </si>
-  <si>
-    <t>Dobias Cole-Truten</t>
-  </si>
-  <si>
-    <t>Killi Gimm</t>
-  </si>
-  <si>
-    <t>Serchill Rostok</t>
-  </si>
-  <si>
-    <t>Torius Chord</t>
+    <t>Baze Malbus</t>
+  </si>
+  <si>
+    <t>Toshma Jefkin</t>
+  </si>
+  <si>
+    <t>Cycyed Ock</t>
+  </si>
+  <si>
+    <t>Jimmon Arbmab</t>
+  </si>
+  <si>
+    <t>Bor Gullet</t>
+  </si>
+  <si>
+    <t>Criden Valdas</t>
+  </si>
+  <si>
+    <t>Ponda Baba</t>
+  </si>
+  <si>
+    <t>Calum Gram</t>
+  </si>
+  <si>
+    <t>Sotorus Ramda</t>
+  </si>
+  <si>
+    <t>Caysin Bog</t>
+  </si>
+  <si>
+    <t>Yosh Calfor</t>
+  </si>
+  <si>
+    <t>Wion Dillems</t>
+  </si>
+  <si>
+    <t>Tivik's sister</t>
+  </si>
+  <si>
+    <t>Unidentified male rebel technician</t>
+  </si>
+  <si>
+    <t>Warda Gojun</t>
+  </si>
+  <si>
+    <t>Kent Deezling</t>
+  </si>
+  <si>
+    <t>Wona Goban</t>
+  </si>
+  <si>
+    <t>Cornelius Evazan</t>
+  </si>
+  <si>
+    <t>Unidentified Rebel MP</t>
+  </si>
+  <si>
+    <t>Gazdo Woolcob</t>
+  </si>
+  <si>
+    <t>K-OHN</t>
+  </si>
+  <si>
+    <t>Oolin Musters</t>
+  </si>
+  <si>
+    <t>Unidentified prisoner (Wobani)</t>
+  </si>
+  <si>
+    <t>Milton Putna</t>
+  </si>
+  <si>
+    <t>Tam Posla</t>
+  </si>
+  <si>
+    <t>Darth Vader</t>
+  </si>
+  <si>
+    <t>Fassio Ablund</t>
+  </si>
+  <si>
+    <t>Bail Organa</t>
+  </si>
+  <si>
+    <t>LU-28</t>
+  </si>
+  <si>
+    <t>TK-40121</t>
+  </si>
+  <si>
+    <t>Lyra Erso</t>
+  </si>
+  <si>
+    <t>Antoc Merrick</t>
+  </si>
+  <si>
+    <t>R3-S1</t>
+  </si>
+  <si>
+    <t>Orson Callan Krennic</t>
+  </si>
+  <si>
+    <t>Caitken</t>
+  </si>
+  <si>
+    <t>Broan Danurs</t>
+  </si>
+  <si>
+    <t>Benthic</t>
+  </si>
+  <si>
+    <t>Arro Basteren</t>
+  </si>
+  <si>
+    <t>TK-1016</t>
+  </si>
+  <si>
+    <t>Darth Sidious</t>
+  </si>
+  <si>
+    <t>Capin Harinar</t>
+  </si>
+  <si>
+    <t>Galen Walton Erso</t>
+  </si>
+  <si>
+    <t>Euwood Gor</t>
+  </si>
+  <si>
+    <t>R5-SK1</t>
+  </si>
+  <si>
+    <t>Bozeden Jeems</t>
+  </si>
+  <si>
+    <t>Moroff</t>
+  </si>
+  <si>
+    <t>Barion Raner</t>
+  </si>
+  <si>
+    <t>Pedrin Gaul</t>
+  </si>
+  <si>
+    <t>The High Priest</t>
+  </si>
+  <si>
+    <t>Davits Draven</t>
+  </si>
+  <si>
+    <t>Kado Oquoné</t>
+  </si>
+  <si>
+    <t>Shaef Corssin</t>
+  </si>
+  <si>
+    <t>Leevan Tenza</t>
   </si>
   <si>
     <t>Stordan Tonc</t>
   </si>
   <si>
-    <t>TK-14057</t>
-  </si>
-  <si>
-    <t>Jek Tono Porkins</t>
-  </si>
-  <si>
-    <t>Casido</t>
-  </si>
-  <si>
-    <t>Dunstig Pterro</t>
-  </si>
-  <si>
-    <t>Datchi Creel</t>
-  </si>
-  <si>
-    <t>Bandwin Cor</t>
-  </si>
-  <si>
-    <t>R3-M2</t>
-  </si>
-  <si>
-    <t>Riss Clyos</t>
-  </si>
-  <si>
-    <t>Tivik</t>
-  </si>
-  <si>
-    <t>Farsin Kappehl</t>
-  </si>
-  <si>
-    <t>Gavra Ubrento</t>
-  </si>
-  <si>
-    <t>Has Obitt</t>
-  </si>
-  <si>
-    <t>Garven Dreis</t>
-  </si>
-  <si>
-    <t>Niles Gavla</t>
-  </si>
-  <si>
-    <t>Chirrut Îmwe</t>
-  </si>
-  <si>
-    <t>Farns Monsbee</t>
+    <t>Unidentified Shield Gate officer</t>
   </si>
   <si>
     <t>Frobb</t>
   </si>
   <si>
-    <t>Baze Malbus</t>
-  </si>
-  <si>
-    <t>Toshma Jefkin</t>
-  </si>
-  <si>
-    <t>Cycyed Ock</t>
-  </si>
-  <si>
-    <t>Jimmon Arbmab</t>
+    <t>Ansin Thobel</t>
+  </si>
+  <si>
+    <t>Kullbee Sperado</t>
+  </si>
+  <si>
+    <t>R2-BHD</t>
+  </si>
+  <si>
+    <t>Huika Siliu</t>
+  </si>
+  <si>
+    <t>Haxen Delto</t>
+  </si>
+  <si>
+    <t>G2-1B7</t>
+  </si>
+  <si>
+    <t>Vlex Onopin</t>
+  </si>
+  <si>
+    <t>Hurst Romodi</t>
+  </si>
+  <si>
+    <t>Dustil Forell</t>
+  </si>
+  <si>
+    <t>Jon Vander</t>
+  </si>
+  <si>
+    <t>Mennis Duren</t>
+  </si>
+  <si>
+    <t>Silvanie Phest</t>
+  </si>
+  <si>
+    <t>Essie</t>
+  </si>
+  <si>
+    <t>Lucky Hazz Obloobitt</t>
+  </si>
+  <si>
+    <t>Wedge Antilles</t>
   </si>
   <si>
     <t>Mon Mothma</t>
-  </si>
-  <si>
-    <t>Bor Gullet</t>
-  </si>
-  <si>
-    <t>Criden Valdas</t>
-  </si>
-  <si>
-    <t>Ponda Baba</t>
-  </si>
-  <si>
-    <t>Calum Gram</t>
-  </si>
-  <si>
-    <t>Sotorus Ramda</t>
-  </si>
-  <si>
-    <t>Caysin Bog</t>
-  </si>
-  <si>
-    <t>Yosh Calfor</t>
-  </si>
-  <si>
-    <t>Wion Dillems</t>
-  </si>
-  <si>
-    <t>Tivik's sister</t>
-  </si>
-  <si>
-    <t>Unidentified male rebel technician</t>
-  </si>
-  <si>
-    <t>Warda Gojun</t>
-  </si>
-  <si>
-    <t>Kent Deezling</t>
-  </si>
-  <si>
-    <t>Wona Goban</t>
-  </si>
-  <si>
-    <t>Cornelius Evazan</t>
-  </si>
-  <si>
-    <t>Unidentified Rebel MP</t>
-  </si>
-  <si>
-    <t>Gazdo Woolcob</t>
-  </si>
-  <si>
-    <t>K-OHN</t>
-  </si>
-  <si>
-    <t>Oolin Musters</t>
-  </si>
-  <si>
-    <t>Unidentified prisoner (Wobani)</t>
-  </si>
-  <si>
-    <t>Milton Putna</t>
-  </si>
-  <si>
-    <t>Tam Posla</t>
-  </si>
-  <si>
-    <t>Darth Vader</t>
-  </si>
-  <si>
-    <t>Fassio Ablund</t>
-  </si>
-  <si>
-    <t>Bail Organa</t>
-  </si>
-  <si>
-    <t>LU-28</t>
-  </si>
-  <si>
-    <t>TK-40121</t>
-  </si>
-  <si>
-    <t>Lyra Erso</t>
-  </si>
-  <si>
-    <t>Antoc Merrick</t>
-  </si>
-  <si>
-    <t>R3-S1</t>
-  </si>
-  <si>
-    <t>Orson Callan Krennic</t>
-  </si>
-  <si>
-    <t>Caitken</t>
-  </si>
-  <si>
-    <t>Broan Danurs</t>
-  </si>
-  <si>
-    <t>Benthic</t>
-  </si>
-  <si>
-    <t>Arro Basteren</t>
-  </si>
-  <si>
-    <t>TK-1016</t>
-  </si>
-  <si>
-    <t>Darth Sidious</t>
-  </si>
-  <si>
-    <t>Capin Harinar</t>
-  </si>
-  <si>
-    <t>Galen Walton Erso</t>
-  </si>
-  <si>
-    <t>Euwood Gor</t>
-  </si>
-  <si>
-    <t>R5-SK1</t>
-  </si>
-  <si>
-    <t>Bozeden Jeems</t>
-  </si>
-  <si>
-    <t>Moroff</t>
-  </si>
-  <si>
-    <t>Barion Raner</t>
-  </si>
-  <si>
-    <t>Pedrin Gaul</t>
-  </si>
-  <si>
-    <t>The High Priest</t>
-  </si>
-  <si>
-    <t>Davits Draven</t>
-  </si>
-  <si>
-    <t>Kado Oquoné</t>
-  </si>
-  <si>
-    <t>Shaef Corssin</t>
-  </si>
-  <si>
-    <t>Leevan Tenza</t>
-  </si>
-  <si>
-    <t>Unidentified Shield Gate officer</t>
-  </si>
-  <si>
-    <t>Ansin Thobel</t>
-  </si>
-  <si>
-    <t>Kullbee Sperado</t>
-  </si>
-  <si>
-    <t>Huika Siliu</t>
-  </si>
-  <si>
-    <t>Haxen Delto</t>
-  </si>
-  <si>
-    <t>G2-1B7</t>
-  </si>
-  <si>
-    <t>Vlex Onopin</t>
-  </si>
-  <si>
-    <t>Hurst Romodi</t>
-  </si>
-  <si>
-    <t>Attico Wred</t>
-  </si>
-  <si>
-    <t>Dustil Forell</t>
-  </si>
-  <si>
-    <t>Jon Vander</t>
-  </si>
-  <si>
-    <t>Mennis Duren</t>
-  </si>
-  <si>
-    <t>Silvanie Phest</t>
-  </si>
-  <si>
-    <t>Essie</t>
-  </si>
-  <si>
-    <t>Lucky Hazz Obloobitt</t>
-  </si>
-  <si>
-    <t>Wedge Antilles</t>
-  </si>
-  <si>
-    <t>R2-BHD</t>
   </si>
   <si>
     <t>Hera Syndulla</t>
@@ -972,7 +972,7 @@
         <v>0.1404494382022472</v>
       </c>
       <c r="E2">
-        <v>0.1745039368149969</v>
+        <v>0.174503936814997</v>
       </c>
       <c r="F2">
         <v>11</v>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1015,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.01869475990661046</v>
+        <v>0.01869475990661045</v>
       </c>
       <c r="C4">
         <v>45</v>
@@ -1024,7 +1024,7 @@
         <v>0.252808988764045</v>
       </c>
       <c r="E4">
-        <v>0.2852353780321321</v>
+        <v>0.2852353780321322</v>
       </c>
       <c r="F4">
         <v>28</v>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1076,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1102,7 +1102,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E7">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1128,7 +1128,7 @@
         <v>0.005617977528089887</v>
       </c>
       <c r="E8">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1154,7 +1154,7 @@
         <v>0.03370786516853932</v>
       </c>
       <c r="E9">
-        <v>2.764031481728775e-19</v>
+        <v>2.764031481728776e-19</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1206,7 +1206,7 @@
         <v>0.2359550561797753</v>
       </c>
       <c r="E11">
-        <v>0.150345235731732</v>
+        <v>0.1503452357317321</v>
       </c>
       <c r="F11">
         <v>31</v>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1258,7 +1258,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E13">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1310,7 +1310,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E15">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1336,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1362,7 +1362,7 @@
         <v>0.1741573033707865</v>
       </c>
       <c r="E17">
-        <v>0.09974206134020995</v>
+        <v>0.09974206134020996</v>
       </c>
       <c r="F17">
         <v>21</v>
@@ -1405,7 +1405,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.0003410508239445551</v>
+        <v>0.000341050823944555</v>
       </c>
       <c r="C19">
         <v>12</v>
@@ -1414,7 +1414,7 @@
         <v>0.06741573033707865</v>
       </c>
       <c r="E19">
-        <v>0.08039623709334941</v>
+        <v>0.08039623709334942</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -1440,7 +1440,7 @@
         <v>0.02808988764044944</v>
       </c>
       <c r="E20">
-        <v>4.146045904600246e-19</v>
+        <v>4.146045904600247e-19</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1466,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1518,7 +1518,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E23">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1570,7 +1570,7 @@
         <v>0.101123595505618</v>
       </c>
       <c r="E25">
-        <v>0.01732735618360601</v>
+        <v>0.01732735618360602</v>
       </c>
       <c r="F25">
         <v>5</v>
@@ -1596,7 +1596,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E26">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1622,7 +1622,7 @@
         <v>0.01685393258426966</v>
       </c>
       <c r="E27">
-        <v>0.007772284942399107</v>
+        <v>0.007772284942399108</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1648,7 +1648,7 @@
         <v>0.005617977528089887</v>
       </c>
       <c r="E28">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1665,7 +1665,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.08578286198048041</v>
+        <v>0.08578286198048039</v>
       </c>
       <c r="C29">
         <v>74</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1752,7 +1752,7 @@
         <v>0.005617977528089887</v>
       </c>
       <c r="E32">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1769,25 +1769,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>3.926620999559488e-05</v>
+        <v>0.06550950769181992</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D33">
-        <v>0.03370786516853932</v>
+        <v>0.3707865168539326</v>
       </c>
       <c r="E33">
-        <v>0.05669334425316937</v>
+        <v>0.2934265187370587</v>
       </c>
       <c r="F33">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
         <v>38</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1795,25 +1795,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.0655095076918199</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0.3707865168539326</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E34">
-        <v>0.2934265187370588</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F34">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="G34" t="s">
         <v>39</v>
       </c>
       <c r="H34">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1824,22 +1824,22 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>0.005617977528089887</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E35">
-        <v>1.317992916931522e-25</v>
+        <v>2.764031481728776e-19</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="s">
         <v>40</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1850,13 +1850,13 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>0.01685393258426966</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E36">
-        <v>2.764031481728775e-19</v>
+        <v>2.899584417249349e-24</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1865,7 +1865,7 @@
         <v>41</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1873,25 +1873,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.0009175380813276111</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D37">
-        <v>0.005617977528089887</v>
+        <v>0.08426966292134831</v>
       </c>
       <c r="E37">
-        <v>2.899584417249348e-24</v>
+        <v>0.01606753785772123</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
         <v>42</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1899,25 +1899,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.0009175380813276112</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>0.08426966292134831</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E38">
-        <v>0.01606753785772123</v>
+        <v>2.899584417249349e-24</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" t="s">
         <v>43</v>
       </c>
       <c r="H38">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1928,13 +1928,13 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39">
-        <v>0.005617977528089887</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E39">
-        <v>2.899584417249348e-24</v>
+        <v>0.0009013092738478578</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1943,7 +1943,7 @@
         <v>44</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1960,16 +1960,16 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E40">
-        <v>0.0009013092738478575</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="s">
         <v>45</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1980,13 +1980,13 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0.01123595505617977</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1995,7 +1995,7 @@
         <v>46</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2003,25 +2003,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.0103358796013052</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>0.1685393258426966</v>
       </c>
       <c r="E42">
-        <v>1.317992916931522e-25</v>
+        <v>0.1597953406775861</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G42" t="s">
         <v>47</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2029,25 +2029,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.0103358796013052</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>0.1685393258426966</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E43">
-        <v>0.1597953406775861</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F43">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G43" t="s">
         <v>48</v>
       </c>
       <c r="H43">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2055,25 +2055,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.006456496410412239</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D44">
-        <v>0.01685393258426966</v>
+        <v>0.1460674157303371</v>
       </c>
       <c r="E44">
-        <v>1.317992916931522e-25</v>
+        <v>0.2149187222318768</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G44" t="s">
         <v>49</v>
       </c>
       <c r="H44">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2081,25 +2081,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.006456496410412241</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>0.1460674157303371</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E45">
-        <v>0.2149187222318768</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F45">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G45" t="s">
         <v>50</v>
       </c>
       <c r="H45">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2107,25 +2107,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>0.0037603993380488</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D46">
-        <v>0.005617977528089887</v>
+        <v>0.1573033707865168</v>
       </c>
       <c r="E46">
-        <v>1.317992916931522e-25</v>
+        <v>0.2065431575309268</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G46" t="s">
         <v>51</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2133,25 +2133,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.0037603993380488</v>
+        <v>0.006563991881074342</v>
       </c>
       <c r="C47">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D47">
-        <v>0.1573033707865168</v>
+        <v>0.03932584269662921</v>
       </c>
       <c r="E47">
-        <v>0.2065431575309267</v>
+        <v>0.001358555468469074</v>
       </c>
       <c r="F47">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G47" t="s">
         <v>52</v>
       </c>
       <c r="H47">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2159,25 +2159,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.006563991881074342</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0.03932584269662921</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>0.001358555468469073</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G48" t="s">
         <v>53</v>
       </c>
       <c r="H48">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2188,22 +2188,22 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E49">
-        <v>1.317992916931522e-25</v>
+        <v>0.03148877632643938</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49" t="s">
         <v>54</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2214,22 +2214,22 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0.02808988764044944</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>0.03148877632643938</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G50" t="s">
         <v>55</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2240,13 +2240,13 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E51">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2255,7 +2255,7 @@
         <v>56</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2263,19 +2263,19 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.004094458198438393</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <v>0.005617977528089887</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E52">
-        <v>1.317992916931522e-25</v>
+        <v>0.0009068143688733751</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52" t="s">
         <v>57</v>
@@ -2289,25 +2289,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.004094458198438393</v>
+        <v>0.01692730234734168</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D53">
-        <v>0.01685393258426966</v>
+        <v>0.2078651685393259</v>
       </c>
       <c r="E53">
-        <v>0.0009068143688733749</v>
+        <v>0.2606298883088305</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="G53" t="s">
         <v>58</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2315,25 +2315,25 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.01692730234734168</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="D54">
-        <v>0.2078651685393259</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E54">
-        <v>0.2606298883088305</v>
+        <v>0.02921233746211352</v>
       </c>
       <c r="F54">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="G54" t="s">
         <v>59</v>
       </c>
       <c r="H54">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2350,7 +2350,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E55">
-        <v>0.02921233746211352</v>
+        <v>0.001350303569529463</v>
       </c>
       <c r="F55">
         <v>2</v>
@@ -2370,22 +2370,22 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <v>0.01123595505617977</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E56">
-        <v>0.001350303569529462</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G56" t="s">
         <v>61</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2393,25 +2393,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.01771896357451128</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D57">
-        <v>0.005617977528089887</v>
+        <v>0.1853932584269663</v>
       </c>
       <c r="E57">
-        <v>1.317992916931522e-25</v>
+        <v>0.1523602433937337</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G57" t="s">
         <v>62</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2419,25 +2419,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.01771896357451128</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D58">
-        <v>0.1853932584269663</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E58">
-        <v>0.1523602433937336</v>
+        <v>0.02921233746211352</v>
       </c>
       <c r="F58">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G58" t="s">
         <v>63</v>
       </c>
       <c r="H58">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2448,13 +2448,13 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D59">
-        <v>0.02808988764044944</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E59">
-        <v>0.02921233746211352</v>
+        <v>0.0277669793215607</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -2463,7 +2463,7 @@
         <v>64</v>
       </c>
       <c r="H59">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2474,22 +2474,22 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>0.02247191011235955</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>0.0277669793215607</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G60" t="s">
         <v>65</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2497,25 +2497,25 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.0009895978756263089</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>0.1235955056179775</v>
       </c>
       <c r="E61">
-        <v>1.317992916931522e-25</v>
+        <v>0.1818981639249554</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G61" t="s">
         <v>66</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2523,25 +2523,25 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.0009895978756263087</v>
+        <v>5.375451480955196e-05</v>
       </c>
       <c r="C62">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D62">
-        <v>0.1235955056179775</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E62">
-        <v>0.1818981639249553</v>
+        <v>4.146047222593164e-19</v>
       </c>
       <c r="F62">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G62" t="s">
         <v>67</v>
       </c>
       <c r="H62">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2549,25 +2549,25 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>5.375451480955196e-05</v>
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D63">
-        <v>0.01685393258426966</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E63">
-        <v>4.146047222593163e-19</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G63" t="s">
         <v>68</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2584,7 +2584,7 @@
         <v>0.02247191011235955</v>
       </c>
       <c r="E64">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2601,25 +2601,25 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.0008721617332886604</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D65">
-        <v>0.02247191011235955</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="E65">
-        <v>1.317992916931522e-25</v>
+        <v>0.07576805364181191</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G65" t="s">
         <v>70</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2627,25 +2627,25 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.0008721617332886604</v>
+        <v>0.009016112054502286</v>
       </c>
       <c r="C66">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D66">
-        <v>0.07865168539325842</v>
+        <v>0.1348314606741573</v>
       </c>
       <c r="E66">
-        <v>0.07576805364181191</v>
+        <v>0.04982452418004565</v>
       </c>
       <c r="F66">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s">
         <v>71</v>
       </c>
       <c r="H66">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2653,25 +2653,25 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.009016112054502288</v>
+        <v>3.926620999559488e-05</v>
       </c>
       <c r="C67">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D67">
-        <v>0.1348314606741573</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="E67">
-        <v>0.04982452418004565</v>
+        <v>0.05669334425316937</v>
       </c>
       <c r="F67">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G67" t="s">
         <v>72</v>
       </c>
       <c r="H67">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2679,19 +2679,19 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.00247571891068368</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68">
-        <v>0.02808988764044944</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E68">
-        <v>0.01596105822744614</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G68" t="s">
         <v>73</v>
@@ -2708,13 +2708,13 @@
         <v>0</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>0.01685393258426966</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2723,7 +2723,7 @@
         <v>74</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2734,13 +2734,13 @@
         <v>0</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E70">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2749,7 +2749,7 @@
         <v>75</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2760,22 +2760,22 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D71">
-        <v>0.005617977528089887</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E71">
-        <v>1.317992916931522e-25</v>
+        <v>0.02921233746211352</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G71" t="s">
         <v>76</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2786,22 +2786,22 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D72">
-        <v>0.02808988764044944</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E72">
-        <v>0.02921233746211352</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G72" t="s">
         <v>77</v>
       </c>
       <c r="H72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2812,13 +2812,13 @@
         <v>0</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>0.02247191011235955</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -2827,7 +2827,7 @@
         <v>78</v>
       </c>
       <c r="H73">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2844,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -2864,13 +2864,13 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E75">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -2879,7 +2879,7 @@
         <v>80</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2887,25 +2887,25 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.002507458896718085</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D76">
-        <v>0.005617977528089887</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E76">
-        <v>1.317992916931522e-25</v>
+        <v>0.02286520119769301</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G76" t="s">
         <v>81</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2913,25 +2913,25 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.002507458896718085</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>0.02808988764044944</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>0.022865201197693</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G77" t="s">
         <v>82</v>
       </c>
       <c r="H77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2948,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -2968,22 +2968,22 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E79">
-        <v>1.317992916931522e-25</v>
+        <v>7.065661526554515e-05</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" t="s">
         <v>84</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2994,22 +2994,22 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>0.02247191011235955</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>0.002218344915075208</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F80">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G80" t="s">
         <v>85</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3017,25 +3017,25 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>0.01458452358280962</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="E81">
-        <v>1.317992916931522e-25</v>
+        <v>0.0115671335275733</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G81" t="s">
         <v>86</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3043,25 +3043,25 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.01458452358280962</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D82">
-        <v>0.03370786516853932</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E82">
-        <v>0.01156713352757329</v>
+        <v>2.764031481728776e-19</v>
       </c>
       <c r="F82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G82" t="s">
         <v>87</v>
       </c>
       <c r="H82">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3072,16 +3072,16 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83">
-        <v>0.01123595505617977</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E83">
-        <v>2.764031481728775e-19</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" t="s">
         <v>88</v>
@@ -3098,13 +3098,13 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>0.005617977528089887</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         <v>89</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3121,25 +3121,25 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>0.002117230333631768</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>0.05056179775280899</v>
       </c>
       <c r="E85">
-        <v>1.317992916931522e-25</v>
+        <v>0.02179183254323248</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" t="s">
         <v>90</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3147,25 +3147,25 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.002117230333631768</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>0.05056179775280899</v>
+        <v>0</v>
       </c>
       <c r="E86">
-        <v>0.02179183254323248</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86" t="s">
         <v>91</v>
       </c>
       <c r="H86">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -3199,25 +3199,25 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>0.0002521458101347646</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E88">
-        <v>1.317992916931522e-25</v>
+        <v>0.01171592283355916</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G88" t="s">
         <v>93</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3225,25 +3225,25 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.0002521458101347646</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>0.02808988764044944</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>0.01171592283355916</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F89">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G89" t="s">
         <v>94</v>
       </c>
       <c r="H89">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3254,13 +3254,13 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E90">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -3269,7 +3269,7 @@
         <v>95</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3277,25 +3277,25 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>0.004345837082738738</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D91">
-        <v>0.005617977528089887</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="E91">
-        <v>1.317992916931522e-25</v>
+        <v>0.09509163802886898</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G91" t="s">
         <v>96</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3303,25 +3303,25 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.004345837082738738</v>
+        <v>0.01588372630287542</v>
       </c>
       <c r="C92">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D92">
-        <v>0.07865168539325842</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="E92">
-        <v>0.09509163802886897</v>
+        <v>0.03404109717363966</v>
       </c>
       <c r="F92">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G92" t="s">
         <v>97</v>
       </c>
       <c r="H92">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3329,25 +3329,25 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.01588372630287542</v>
+        <v>0</v>
       </c>
       <c r="C93">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>0.0898876404494382</v>
+        <v>0</v>
       </c>
       <c r="E93">
-        <v>0.03404109717363966</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F93">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G93" t="s">
         <v>98</v>
       </c>
       <c r="H93">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3355,25 +3355,25 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>0.006301395190021097</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>0.1292134831460674</v>
       </c>
       <c r="E94">
-        <v>1.317992916931522e-25</v>
+        <v>0.08497844106716748</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G94" t="s">
         <v>99</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3381,25 +3381,25 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.006301395190021099</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D95">
-        <v>0.1292134831460674</v>
+        <v>0.03932584269662921</v>
       </c>
       <c r="E95">
-        <v>0.08497844106716747</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F95">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G95" t="s">
         <v>100</v>
       </c>
       <c r="H95">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3407,25 +3407,25 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>0.00247571891068368</v>
       </c>
       <c r="C96">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D96">
-        <v>0.03932584269662921</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E96">
-        <v>1.317992916931522e-25</v>
+        <v>0.01596105822744615</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G96" t="s">
         <v>101</v>
       </c>
       <c r="H96">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3433,25 +3433,25 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>0.006599838402998772</v>
       </c>
       <c r="C97">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D97">
-        <v>0.02247191011235955</v>
+        <v>0.1179775280898876</v>
       </c>
       <c r="E97">
-        <v>1.317992916931522e-25</v>
+        <v>0.08497844106716748</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G97" t="s">
         <v>102</v>
       </c>
       <c r="H97">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -3459,25 +3459,25 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.006599838402998771</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D98">
-        <v>0.1179775280898876</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E98">
-        <v>0.08497844106716747</v>
+        <v>0.02179183254323248</v>
       </c>
       <c r="F98">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G98" t="s">
         <v>103</v>
       </c>
       <c r="H98">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3488,16 +3488,16 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D99">
-        <v>0.02808988764044944</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E99">
-        <v>0.02179183254323248</v>
+        <v>2.764031481728776e-19</v>
       </c>
       <c r="F99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G99" t="s">
         <v>104</v>
@@ -3511,16 +3511,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>0.002539198882752492</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D100">
-        <v>0.02247191011235955</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E100">
-        <v>2.764031481728775e-19</v>
+        <v>2.899584417249349e-24</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3529,7 +3529,7 @@
         <v>105</v>
       </c>
       <c r="H100">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3537,25 +3537,25 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.002539198882752492</v>
+        <v>0</v>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D101">
-        <v>0.01685393258426966</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E101">
-        <v>2.899584417249348e-24</v>
+        <v>0.03473812487436079</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G101" t="s">
         <v>106</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3563,25 +3563,25 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.03210692093490439</v>
+        <v>0</v>
       </c>
       <c r="C102">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D102">
-        <v>0.247191011235955</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E102">
-        <v>0.2565957332176505</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F102">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G102" t="s">
         <v>107</v>
       </c>
       <c r="H102">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3589,25 +3589,25 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>0.0007004333013664568</v>
       </c>
       <c r="C103">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D103">
-        <v>0.02808988764044944</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="E103">
-        <v>0.03473812487436079</v>
+        <v>0.02490130194061032</v>
       </c>
       <c r="F103">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G103" t="s">
         <v>108</v>
       </c>
       <c r="H103">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3618,13 +3618,13 @@
         <v>0</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>0.005617977528089887</v>
+        <v>0</v>
       </c>
       <c r="E104">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -3633,7 +3633,7 @@
         <v>109</v>
       </c>
       <c r="H104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3641,7 +3641,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.0007004333013664568</v>
+        <v>0.004178280671771155</v>
       </c>
       <c r="C105">
         <v>10</v>
@@ -3650,16 +3650,16 @@
         <v>0.05617977528089887</v>
       </c>
       <c r="E105">
-        <v>0.02490130194061031</v>
+        <v>0.01358964632340206</v>
       </c>
       <c r="F105">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G105" t="s">
         <v>110</v>
       </c>
       <c r="H105">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3667,25 +3667,25 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>0.000213975253253486</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>0.0449438202247191</v>
       </c>
       <c r="E106">
-        <v>1.317992916931522e-25</v>
+        <v>0.02355865654457568</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G106" t="s">
         <v>111</v>
       </c>
       <c r="H106">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3693,25 +3693,25 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0.004178280671771155</v>
+        <v>0</v>
       </c>
       <c r="C107">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D107">
-        <v>0.05617977528089887</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E107">
-        <v>0.01358964632340206</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F107">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G107" t="s">
         <v>112</v>
       </c>
       <c r="H107">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3719,25 +3719,25 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.000213975253253486</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>0.0449438202247191</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>0.02355865654457569</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F108">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G108" t="s">
         <v>113</v>
       </c>
       <c r="H108">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3748,13 +3748,13 @@
         <v>0</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D109">
-        <v>0.005617977528089887</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E109">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>114</v>
       </c>
       <c r="H109">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3774,13 +3774,13 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E110">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3789,7 +3789,7 @@
         <v>115</v>
       </c>
       <c r="H110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3800,13 +3800,13 @@
         <v>0</v>
       </c>
       <c r="C111">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D111">
-        <v>0.02247191011235955</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E111">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -3815,7 +3815,7 @@
         <v>116</v>
       </c>
       <c r="H111">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3832,7 +3832,7 @@
         <v>0.005617977528089887</v>
       </c>
       <c r="E112">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -3852,13 +3852,13 @@
         <v>0</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D113">
-        <v>0.005617977528089887</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E113">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -3867,7 +3867,7 @@
         <v>118</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3875,25 +3875,25 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>0.002172779535735246</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D114">
-        <v>0.005617977528089887</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="E114">
-        <v>1.317992916931522e-25</v>
+        <v>0.06077970307124594</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G114" t="s">
         <v>119</v>
       </c>
       <c r="H114">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3904,13 +3904,13 @@
         <v>0</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>0.01685393258426966</v>
+        <v>0</v>
       </c>
       <c r="E115">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -3919,7 +3919,7 @@
         <v>120</v>
       </c>
       <c r="H115">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3927,25 +3927,25 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.002172779535735246</v>
+        <v>0</v>
       </c>
       <c r="C116">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>0.07865168539325842</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>0.06077970307124595</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F116">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G116" t="s">
         <v>121</v>
       </c>
       <c r="H116">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -3982,22 +3982,22 @@
         <v>0</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E118">
-        <v>1.317992916931522e-25</v>
+        <v>0.01471723428819176</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G118" t="s">
         <v>123</v>
       </c>
       <c r="H118">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4008,22 +4008,22 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E119">
-        <v>1.317992916931522e-25</v>
+        <v>0.001350303569529463</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119" t="s">
         <v>124</v>
       </c>
       <c r="H119">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4034,10 +4034,10 @@
         <v>0</v>
       </c>
       <c r="C120">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D120">
-        <v>0.02808988764044944</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E120">
         <v>0.01471723428819176</v>
@@ -4049,7 +4049,7 @@
         <v>125</v>
       </c>
       <c r="H120">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4057,25 +4057,25 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>0.000318799076178623</v>
       </c>
       <c r="C121">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D121">
-        <v>0.01685393258426966</v>
+        <v>0.05056179775280899</v>
       </c>
       <c r="E121">
-        <v>0.001350303569529462</v>
+        <v>0.02355865654457568</v>
       </c>
       <c r="F121">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G121" t="s">
         <v>126</v>
       </c>
       <c r="H121">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4083,25 +4083,25 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>0.04947118158055006</v>
       </c>
       <c r="C122">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D122">
-        <v>0.02247191011235955</v>
+        <v>0.2696629213483146</v>
       </c>
       <c r="E122">
-        <v>0.01471723428819176</v>
+        <v>0.2796609445082329</v>
       </c>
       <c r="F122">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G122" t="s">
         <v>127</v>
       </c>
       <c r="H122">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4109,25 +4109,25 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>0.000318799076178623</v>
+        <v>0</v>
       </c>
       <c r="C123">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D123">
-        <v>0.05056179775280899</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E123">
-        <v>0.02355865654457568</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F123">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G123" t="s">
         <v>128</v>
       </c>
       <c r="H123">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4135,25 +4135,25 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>0.04947118158055006</v>
+        <v>0.005871915065302179</v>
       </c>
       <c r="C124">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D124">
-        <v>0.2696629213483146</v>
+        <v>0.1741573033707865</v>
       </c>
       <c r="E124">
-        <v>0.2796609445082328</v>
+        <v>0.2326337043038795</v>
       </c>
       <c r="F124">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G124" t="s">
         <v>129</v>
       </c>
       <c r="H124">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4164,13 +4164,13 @@
         <v>0</v>
       </c>
       <c r="C125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>0.005617977528089887</v>
+        <v>0</v>
       </c>
       <c r="E125">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F125">
         <v>0</v>
@@ -4179,7 +4179,7 @@
         <v>130</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -4187,25 +4187,25 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>0.00587191506530218</v>
+        <v>0</v>
       </c>
       <c r="C126">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="D126">
-        <v>0.1741573033707865</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E126">
-        <v>0.2326337043038794</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F126">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G126" t="s">
         <v>131</v>
       </c>
       <c r="H126">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -4213,25 +4213,25 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>0.0004011598668090843</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="E127">
-        <v>1.317992916931522e-25</v>
+        <v>0.09509163802886898</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G127" t="s">
         <v>132</v>
       </c>
       <c r="H127">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4239,25 +4239,25 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>0.003466307995645766</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D128">
-        <v>0.005617977528089887</v>
+        <v>0.05056179775280899</v>
       </c>
       <c r="E128">
-        <v>1.317992916931522e-25</v>
+        <v>0.004350568414593132</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G128" t="s">
         <v>133</v>
       </c>
       <c r="H128">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -4265,25 +4265,25 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>0.0004011598668090843</v>
+        <v>0</v>
       </c>
       <c r="C129">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D129">
-        <v>0.07865168539325842</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E129">
-        <v>0.09509163802886897</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F129">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G129" t="s">
         <v>134</v>
       </c>
       <c r="H129">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -4291,25 +4291,25 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>0.003466307995645766</v>
+        <v>0.03447241163483265</v>
       </c>
       <c r="C130">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D130">
-        <v>0.05056179775280899</v>
+        <v>0.2303370786516854</v>
       </c>
       <c r="E130">
-        <v>0.004350568414593132</v>
+        <v>0.1429434928730405</v>
       </c>
       <c r="F130">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G130" t="s">
         <v>135</v>
       </c>
       <c r="H130">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4320,16 +4320,16 @@
         <v>0</v>
       </c>
       <c r="C131">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D131">
-        <v>0.01123595505617977</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E131">
-        <v>1.317992916931522e-25</v>
+        <v>2.764031481728776e-19</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G131" t="s">
         <v>136</v>
@@ -4343,25 +4343,25 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>0.03447241163483265</v>
+        <v>0</v>
       </c>
       <c r="C132">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>0.2303370786516854</v>
+        <v>0</v>
       </c>
       <c r="E132">
-        <v>0.1429434928730405</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F132">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G132" t="s">
         <v>137</v>
       </c>
       <c r="H132">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -4369,25 +4369,25 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>0.002843525668080248</v>
       </c>
       <c r="C133">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D133">
-        <v>0.01685393258426966</v>
+        <v>0.08426966292134831</v>
       </c>
       <c r="E133">
-        <v>2.764031481728775e-19</v>
+        <v>0.06652431969512904</v>
       </c>
       <c r="F133">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G133" t="s">
         <v>138</v>
       </c>
       <c r="H133">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -4398,13 +4398,13 @@
         <v>0</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E134">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F134">
         <v>0</v>
@@ -4413,7 +4413,7 @@
         <v>139</v>
       </c>
       <c r="H134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -4421,25 +4421,25 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>0.00284352566808025</v>
+        <v>0</v>
       </c>
       <c r="C135">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>0.08426966292134831</v>
+        <v>0</v>
       </c>
       <c r="E135">
-        <v>0.06652431969512902</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F135">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G135" t="s">
         <v>140</v>
       </c>
       <c r="H135">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -4447,25 +4447,25 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>0.005004562699577087</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D136">
-        <v>0.005617977528089887</v>
+        <v>0.1629213483146068</v>
       </c>
       <c r="E136">
-        <v>1.317992916931522e-25</v>
+        <v>0.273146590510765</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G136" t="s">
         <v>141</v>
       </c>
       <c r="H136">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -4476,13 +4476,13 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E137">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F137">
         <v>0</v>
@@ -4491,7 +4491,7 @@
         <v>142</v>
       </c>
       <c r="H137">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -4499,25 +4499,25 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>0.005004562699577087</v>
+        <v>0.02571783116239282</v>
       </c>
       <c r="C138">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D138">
-        <v>0.1629213483146068</v>
+        <v>0.2696629213483146</v>
       </c>
       <c r="E138">
-        <v>0.273146590510765</v>
+        <v>0.2319305453745902</v>
       </c>
       <c r="F138">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G138" t="s">
         <v>143</v>
       </c>
       <c r="H138">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -4534,7 +4534,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E139">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F139">
         <v>0</v>
@@ -4551,25 +4551,25 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>0.02571783116239281</v>
+        <v>0</v>
       </c>
       <c r="C140">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D140">
-        <v>0.2696629213483146</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E140">
-        <v>0.2319305453745902</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F140">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="G140" t="s">
         <v>145</v>
       </c>
       <c r="H140">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4580,13 +4580,13 @@
         <v>0</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>0.01123595505617977</v>
+        <v>0</v>
       </c>
       <c r="E141">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F141">
         <v>0</v>
@@ -4595,7 +4595,7 @@
         <v>146</v>
       </c>
       <c r="H141">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4603,25 +4603,25 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>0</v>
+        <v>2.909498719820563e-05</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D142">
-        <v>0.005617977528089887</v>
+        <v>0.03932584269662921</v>
       </c>
       <c r="E142">
-        <v>1.317992916931522e-25</v>
+        <v>0.0184283848236844</v>
       </c>
       <c r="F142">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G142" t="s">
         <v>147</v>
       </c>
       <c r="H142">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4629,25 +4629,25 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>0.0004443598044816859</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E143">
-        <v>1.317992916931522e-25</v>
+        <v>5.667369542805547e-24</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G143" t="s">
         <v>148</v>
       </c>
       <c r="H143">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4655,19 +4655,19 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>2.909498719820563e-05</v>
+        <v>0.003029581666984067</v>
       </c>
       <c r="C144">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D144">
-        <v>0.03932584269662921</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="E144">
-        <v>0.0184283848236844</v>
+        <v>0.002652513704678679</v>
       </c>
       <c r="F144">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G144" t="s">
         <v>149</v>
@@ -4681,25 +4681,25 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>0.0004443598044816859</v>
+        <v>0</v>
       </c>
       <c r="C145">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D145">
-        <v>0.02247191011235955</v>
+        <v>0</v>
       </c>
       <c r="E145">
-        <v>5.667369542805547e-24</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F145">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G145" t="s">
         <v>150</v>
       </c>
       <c r="H145">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4707,25 +4707,25 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>0.003029581666984067</v>
+        <v>0.009347790288476647</v>
       </c>
       <c r="C146">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D146">
-        <v>0.03370786516853932</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="E146">
-        <v>0.002652513704678679</v>
+        <v>0.09690536493529713</v>
       </c>
       <c r="F146">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G146" t="s">
         <v>151</v>
       </c>
       <c r="H146">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4736,13 +4736,13 @@
         <v>0</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="E147">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F147">
         <v>0</v>
@@ -4751,7 +4751,7 @@
         <v>152</v>
       </c>
       <c r="H147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4759,25 +4759,25 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>0.009347790288476647</v>
+        <v>0</v>
       </c>
       <c r="C148">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D148">
-        <v>0.101123595505618</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E148">
-        <v>0.0969053649352971</v>
+        <v>0.02179183254323248</v>
       </c>
       <c r="F148">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G148" t="s">
         <v>153</v>
       </c>
       <c r="H148">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4785,25 +4785,25 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>8.178198998995038e-05</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D149">
-        <v>0.005617977528089887</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E149">
-        <v>1.317992916931522e-25</v>
+        <v>0.01245151917273749</v>
       </c>
       <c r="F149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G149" t="s">
         <v>154</v>
       </c>
       <c r="H149">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -4814,16 +4814,16 @@
         <v>0</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D150">
-        <v>0.01123595505617977</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E150">
-        <v>0.02179183254323248</v>
+        <v>0.002218344915075209</v>
       </c>
       <c r="F150">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G150" t="s">
         <v>155</v>
@@ -4837,25 +4837,25 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>8.178198998995038e-05</v>
+        <v>0</v>
       </c>
       <c r="C151">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D151">
-        <v>0.02247191011235955</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E151">
-        <v>0.01245151917273749</v>
+        <v>0.02659015796485956</v>
       </c>
       <c r="F151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G151" t="s">
         <v>156</v>
       </c>
       <c r="H151">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -4866,22 +4866,22 @@
         <v>0</v>
       </c>
       <c r="C152">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D152">
-        <v>0.01123595505617977</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="E152">
-        <v>0.02659015796485955</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F152">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G152" t="s">
         <v>157</v>
       </c>
       <c r="H152">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4898,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="E153">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F153">
         <v>0</v>
@@ -4924,7 +4924,7 @@
         <v>0.02247191011235955</v>
       </c>
       <c r="E154">
-        <v>2.764031481728775e-19</v>
+        <v>2.764031481728776e-19</v>
       </c>
       <c r="F154">
         <v>1</v>
@@ -4941,25 +4941,25 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>0</v>
+        <v>0.004229759501061208</v>
       </c>
       <c r="C155">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D155">
-        <v>0.01685393258426966</v>
+        <v>0.02808988764044944</v>
       </c>
       <c r="E155">
-        <v>0.01596105822744614</v>
+        <v>0.005280452053035398</v>
       </c>
       <c r="F155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G155" t="s">
         <v>160</v>
       </c>
       <c r="H155">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -4970,22 +4970,22 @@
         <v>0</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E156">
-        <v>1.317992916931522e-25</v>
+        <v>0.01596105822744615</v>
       </c>
       <c r="F156">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G156" t="s">
         <v>161</v>
       </c>
       <c r="H156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4996,13 +4996,13 @@
         <v>0</v>
       </c>
       <c r="C157">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D157">
-        <v>0.01685393258426966</v>
+        <v>0</v>
       </c>
       <c r="E157">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F157">
         <v>0</v>
@@ -5011,7 +5011,7 @@
         <v>162</v>
       </c>
       <c r="H157">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5022,22 +5022,22 @@
         <v>0</v>
       </c>
       <c r="C158">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D158">
-        <v>0.01123595505617977</v>
+        <v>0.01685393258426966</v>
       </c>
       <c r="E158">
-        <v>0.02921233746211352</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F158">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G158" t="s">
         <v>163</v>
       </c>
       <c r="H158">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5045,25 +5045,25 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>0.0004615404063128306</v>
+        <v>0</v>
       </c>
       <c r="C159">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D159">
-        <v>0.06179775280898876</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="E159">
-        <v>0.02030924466491775</v>
+        <v>0.02921233746211352</v>
       </c>
       <c r="F159">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G159" t="s">
         <v>164</v>
       </c>
       <c r="H159">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5071,16 +5071,16 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>0</v>
+        <v>0.0004615404063128306</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D160">
-        <v>0.01123595505617977</v>
+        <v>0.06179775280898876</v>
       </c>
       <c r="E160">
-        <v>7.065661526554513e-05</v>
+        <v>0.02030924466491775</v>
       </c>
       <c r="F160">
         <v>1</v>
@@ -5089,7 +5089,7 @@
         <v>165</v>
       </c>
       <c r="H160">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5106,7 +5106,7 @@
         <v>0</v>
       </c>
       <c r="E161">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F161">
         <v>0</v>
@@ -5132,7 +5132,7 @@
         <v>0.1067415730337079</v>
       </c>
       <c r="E162">
-        <v>0.06776645856583123</v>
+        <v>0.06776645856583122</v>
       </c>
       <c r="F162">
         <v>8</v>
@@ -5158,7 +5158,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E163">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -5184,7 +5184,7 @@
         <v>0.01685393258426966</v>
       </c>
       <c r="E164">
-        <v>2.899584417249348e-24</v>
+        <v>2.899584417249349e-24</v>
       </c>
       <c r="F164">
         <v>1</v>
@@ -5210,7 +5210,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E165">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F165">
         <v>0</v>
@@ -5236,7 +5236,7 @@
         <v>0.02808988764044944</v>
       </c>
       <c r="E166">
-        <v>0.007410157522315189</v>
+        <v>0.007410157522315192</v>
       </c>
       <c r="F166">
         <v>1</v>
@@ -5262,7 +5262,7 @@
         <v>0.1235955056179775</v>
       </c>
       <c r="E167">
-        <v>0.147545102269816</v>
+        <v>0.1475451022698161</v>
       </c>
       <c r="F167">
         <v>10</v>
@@ -5279,25 +5279,25 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>0.004229759501061208</v>
+        <v>0.03210692093490439</v>
       </c>
       <c r="C168">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D168">
-        <v>0.02808988764044944</v>
+        <v>0.247191011235955</v>
       </c>
       <c r="E168">
-        <v>0.005280452053035398</v>
+        <v>0.2565957332176506</v>
       </c>
       <c r="F168">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G168" t="s">
         <v>173</v>
       </c>
       <c r="H168">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -5305,7 +5305,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>0.01376828072835376</v>
+        <v>0.01376828072835377</v>
       </c>
       <c r="C169">
         <v>32</v>
@@ -5340,7 +5340,7 @@
         <v>0</v>
       </c>
       <c r="E170">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -5366,7 +5366,7 @@
         <v>0.01685393258426966</v>
       </c>
       <c r="E171">
-        <v>0.008803461814732865</v>
+        <v>0.008803461814732868</v>
       </c>
       <c r="F171">
         <v>3</v>
@@ -5392,7 +5392,7 @@
         <v>0.005617977528089887</v>
       </c>
       <c r="E172">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F172">
         <v>0</v>
@@ -5418,7 +5418,7 @@
         <v>0.01123595505617977</v>
       </c>
       <c r="E173">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F173">
         <v>0</v>
@@ -5444,7 +5444,7 @@
         <v>0.02247191011235955</v>
       </c>
       <c r="E174">
-        <v>2.899584417249348e-24</v>
+        <v>2.899584417249349e-24</v>
       </c>
       <c r="F174">
         <v>1</v>
@@ -5470,7 +5470,7 @@
         <v>0.05617977528089887</v>
       </c>
       <c r="E175">
-        <v>0.02948743808685214</v>
+        <v>0.02948743808685215</v>
       </c>
       <c r="F175">
         <v>2</v>
@@ -5496,7 +5496,7 @@
         <v>0</v>
       </c>
       <c r="E176">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F176">
         <v>0</v>
@@ -5522,7 +5522,7 @@
         <v>0.005617977528089887</v>
       </c>
       <c r="E177">
-        <v>1.317992916931522e-25</v>
+        <v>1.317992916931523e-25</v>
       </c>
       <c r="F177">
         <v>0</v>
@@ -5548,7 +5548,7 @@
         <v>0.02808988764044944</v>
       </c>
       <c r="E178">
-        <v>6.379085717948565e-23</v>
+        <v>6.379085717948567e-23</v>
       </c>
       <c r="F178">
         <v>3</v>
@@ -5600,7 +5600,7 @@
         <v>0.03932584269662921</v>
       </c>
       <c r="E180">
-        <v>0.01113902951670554</v>
+        <v>0.01113902951670555</v>
       </c>
       <c r="F180">
         <v>2</v>

</xml_diff>